<commit_message>
Rev 3 MM boards and Migration to KICAD
</commit_message>
<xml_diff>
--- a/hw/PCB/EAGLE/MiniMojo_Control_Boards/ATSAMR18_core/ATSAMR18_core_Rev2/TA_bom.xlsx
+++ b/hw/PCB/EAGLE/MiniMojo_Control_Boards/ATSAMR18_core/ATSAMR18_core_Rev2/TA_bom.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27500" windowHeight="21080"/>
+    <workbookView xWindow="300" yWindow="0" windowWidth="16000" windowHeight="21080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -429,7 +429,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -449,6 +449,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -467,8 +483,184 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -482,7 +674,183 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="177">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -814,11 +1182,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A2:A45"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="3" max="3" width="55.83203125" customWidth="1"/>
+    <col min="4" max="4" width="37.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13">
       <c r="A1" s="1" t="s">
@@ -1452,7 +1825,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>